<commit_message>
galacticPubs::publish() [2022-04-24 20:17:52]  added an appeal to do feedback at end of procedure
</commit_message>
<xml_diff>
--- a/meta/procedure_GSheetsOnly.xlsx
+++ b/meta/procedure_GSheetsOnly.xlsx
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="100">
   <si>
     <t>Part</t>
   </si>
@@ -262,7 +262,7 @@
     <t>A quick activity to get students thinking about the behavioral roles that males and females play across the animal kingdom.</t>
   </si>
   <si>
-    <t>Students will pick one of the supplied adjectives and categorize it to one of the sexes, and provide an example of a nonhuman animal that demonstrates this adjective. The idea is to have students think about their preconceptions about *sex roles*. We define it here, but won't introduce the term until part 2. A reason for this is that the utility of the term *sex roles* itself is [being argued about in the scientific literature](https://scholar.google.com/scholar?hl=en&amp;as_sdt=0%2C43&amp;q=On+anisogamy+and+the+evolution+of+%E2%80%98sex+roles%E2%80%99&amp;btnG=&amp;oq=on+anisogamy). 
+    <t>Students will pick one of the supplied adjectives and categorize it to one of the sexes, and provide an example of a nonhuman animal that demonstrates this adjective. The idea is to have students think about their preconceptions about *sex roles*. We define it here for you, but won't introduce this term until part 2. A reason for this is that the utility of the term *sex roles* itself is [being argued about in the scientific literature](https://scholar.google.com/scholar?hl=en&amp;as_sdt=0%2C43&amp;q=On+anisogamy+and+the+evolution+of+%E2%80%98sex+roles%E2%80%99&amp;btnG=&amp;oq=on+anisogamy). 
 We want students to understand that there is a general pattern of how male and female animals tend to behave, but these are not actually prescriptive *roles* and there is a great deal of variation within and across species.</t>
   </si>
   <si>
@@ -352,7 +352,7 @@
     <t>Everything downstream requires that all students collect the data they are introducing. Students will likely need periodic reminders to focus and take down the data to move on. We've added the timers as a reminder.</t>
   </si>
   <si>
-    <t>dewlap=the extendable flap under some lizards (such as the green anole), which is used for competition and mate attraction
+    <t>dewlap=the extendable flap under some lizards' necks (e.g. in green anoles), which is used for competition and mate attraction
 wattle=a fleshy flap of skin on some birds (such as turkeys and jacanas) that likely plays a role in mate choice</t>
   </si>
   <si>
@@ -481,6 +481,9 @@
   </si>
   <si>
     <t>In order to complete the primary task, students will have to compare the units of the X and Y axis on a scatter plot to the values in the table in order to figure out how to label the figure. They will also have to compare the relative values of males and females in order to label the legend key. Once they have figured out the main task, students are asked to interpret whether the data meet criterion 3: that females call more than males (they do). Finally, students are asked to write a persuasive paragraph synthesizing what they have learned to  explain why guardian frogs deserve more research funding and what will be lost if they are allowed to go extinct.</t>
+  </si>
+  <si>
+    <t>When you finish teaching this lesson, we would really love to hear what you thought! Please fill out a simple survey in the Feedback section below.</t>
   </si>
   <si>
     <t>Sequence</t>
@@ -11083,7 +11086,9 @@
       </c>
       <c r="I17" s="35"/>
       <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
+      <c r="K17" s="40" t="s">
+        <v>98</v>
+      </c>
       <c r="M17" s="20"/>
       <c r="N17" s="42"/>
       <c r="O17" s="22" t="s">
@@ -31816,7 +31821,7 @@
         <v>count Part</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" ht="15.0" customHeight="1">

</xml_diff>

<commit_message>
update with Erica's feedback (and changes)
</commit_message>
<xml_diff>
--- a/meta/procedure_GSheetsOnly.xlsx
+++ b/meta/procedure_GSheetsOnly.xlsx
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="101">
   <si>
     <t>Part</t>
   </si>
@@ -481,6 +481,9 @@
   </si>
   <si>
     <t>In order to complete the primary task, students will have to compare the units of the X and Y axis on a scatter plot to the values in the table in order to figure out how to label the figure. They will also have to compare the relative values of males and females in order to label the legend key. Once they have figured out the main task, students are asked to interpret whether the data meet criterion 3: that females call more than males (they do). Finally, students are asked to write a persuasive paragraph synthesizing what they have learned to  explain why guardian frogs deserve more research funding and what will be lost if they are allowed to go extinct.</t>
+  </si>
+  <si>
+    <t>If you'd like to have students refer to outside resources for their final essay, you can assign one of the articles listed in [the Background Section](#background).</t>
   </si>
   <si>
     <t>When you finish teaching this lesson, we would really love to hear what you thought! Please fill out a simple survey in the Feedback section below.</t>
@@ -11085,9 +11088,11 @@
         <v>97</v>
       </c>
       <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="J17" s="40" t="s">
+        <v>98</v>
+      </c>
       <c r="K17" s="40" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M17" s="20"/>
       <c r="N17" s="42"/>
@@ -31821,7 +31826,7 @@
         <v>count Part</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" ht="15.0" customHeight="1">

</xml_diff>